<commit_message>
+ bunch of changes
</commit_message>
<xml_diff>
--- a/002. Input Tables/project_plan.xlsx
+++ b/002. Input Tables/project_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://heinz365-my.sharepoint.com/personal/humberto_consoloholanda_kraftheinz_com/Documents/Documents/GitHub/MSDS460-Assignment_02_/002. Input Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87905A7B-6DAA-40F2-8729-BA8E99DB279F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{87905A7B-6DAA-40F2-8729-BA8E99DB279F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38E3CF8C-31C5-4F24-9918-A09D506FD0E1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2F3D29FD-3600-47DA-87DC-C635DFB0C1D9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
   <si>
     <t>taskID</t>
   </si>
@@ -616,7 +616,7 @@
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,6 +720,18 @@
       <c r="G2">
         <v>1</v>
       </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
       <c r="L2">
         <v>60</v>
       </c>
@@ -764,6 +776,18 @@
       <c r="G3">
         <v>1</v>
       </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
       <c r="L3">
         <v>60</v>
       </c>
@@ -811,6 +835,18 @@
       <c r="G4">
         <v>1</v>
       </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
       <c r="L4">
         <v>60</v>
       </c>
@@ -843,10 +879,31 @@
       <c r="B5" t="s">
         <v>26</v>
       </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
       <c r="D5">
         <v>0</v>
       </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
       <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
@@ -882,7 +939,7 @@
         <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D6">
         <v>40</v>
@@ -1014,8 +1071,14 @@
       <c r="G8">
         <v>1</v>
       </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
       <c r="I8">
         <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -1064,6 +1127,21 @@
       <c r="F9">
         <v>0</v>
       </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
       <c r="L9">
         <v>60</v>
       </c>
@@ -1108,8 +1186,20 @@
       <c r="F10">
         <v>300</v>
       </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
       <c r="H10">
         <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
       </c>
       <c r="L10">
         <v>60</v>
@@ -1155,8 +1245,20 @@
       <c r="F11">
         <v>180</v>
       </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
       <c r="I11">
         <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
       </c>
       <c r="L11">
         <v>60</v>
@@ -1202,8 +1304,20 @@
       <c r="F12">
         <v>120</v>
       </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
       <c r="J12">
         <v>1</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
       </c>
       <c r="L12">
         <v>60</v>
@@ -1249,6 +1363,18 @@
       <c r="F13">
         <v>160</v>
       </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
       <c r="K13">
         <v>1</v>
       </c>
@@ -1296,6 +1422,21 @@
       <c r="F14">
         <v>0</v>
       </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
       <c r="L14">
         <v>60</v>
       </c>
@@ -1399,11 +1540,17 @@
       <c r="F16">
         <v>80</v>
       </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
       <c r="H16">
         <v>1</v>
       </c>
       <c r="I16">
         <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -1461,6 +1608,9 @@
       <c r="I17">
         <v>1</v>
       </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
       <c r="K17">
         <v>1</v>
       </c>
@@ -1570,6 +1720,18 @@
       <c r="G19">
         <v>1</v>
       </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
       <c r="L19">
         <v>60</v>
       </c>
@@ -1617,6 +1779,18 @@
       <c r="G20">
         <v>1</v>
       </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
       <c r="L20">
         <v>60</v>
       </c>
@@ -1664,6 +1838,18 @@
       <c r="G21">
         <v>1</v>
       </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
       <c r="L21">
         <v>60</v>
       </c>
@@ -1710,6 +1896,18 @@
       </c>
       <c r="G22">
         <v>1</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
       </c>
       <c r="L22">
         <v>60</v>

</xml_diff>